<commit_message>
Add title to Drip Box
</commit_message>
<xml_diff>
--- a/docs/report_CaseSummary_1316357068 Mod for Jira Import.xlsx
+++ b/docs/report_CaseSummary_1316357068 Mod for Jira Import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rconover\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rconover\Documents\GitHub\test-station\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F7BDA04-1FAD-49B2-81F9-B3E81D423155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462147C7-5C33-4BBD-9E23-C9D5B2708102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21312" windowHeight="9648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Case Summary" sheetId="1" r:id="rId1"/>
@@ -12776,7 +12776,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -12792,6 +12792,12 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -13315,16 +13321,16 @@
   <dimension ref="A1:P1322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82:D85"/>
+      <pane ySplit="1" topLeftCell="A615" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="39.109375" style="1" customWidth="1"/>
@@ -13332,35 +13338,35 @@
     <col min="21" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" s="11" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -53929,6 +53935,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" verticalDpi="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>